<commit_message>
Cap nhat Activity Bar Chart
</commit_message>
<xml_diff>
--- a/Bao cao/Activity Bar Chart.xlsx
+++ b/Bao cao/Activity Bar Chart.xlsx
@@ -504,13 +504,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="177" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="d"/>
   </numFmts>
   <fonts count="47">
@@ -713,15 +713,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -743,53 +737,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,7 +768,59 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -976,13 +976,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,25 +1054,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,79 +1090,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,15 +1239,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1259,6 +1250,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1278,17 +1287,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1300,6 +1298,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1327,27 +1336,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1355,20 +1355,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1377,85 +1377,85 @@
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="41" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="30" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="30" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1464,22 +1464,22 @@
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1545,10 +1545,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2466,7 +2466,7 @@
   <dimension ref="A1:BL131"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
@@ -12268,7 +12268,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{aa11a8f2-eb39-4805-b857-351575796bf6}</x14:id>
+          <x14:id>{ffe80b8e-6d0e-4556-97a8-da7ee6b14e3a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12282,7 +12282,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{befd2a02-8225-4779-bee9-4a7436c8581b}</x14:id>
+          <x14:id>{1a09c170-6c36-449a-9635-45663dcefaa0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12296,7 +12296,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f5b9f4de-06fd-441a-b84c-d9e8a27b23a3}</x14:id>
+          <x14:id>{3c34237c-1a35-44c0-870d-3b59b76cdda3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12310,7 +12310,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{827e6eec-407e-4811-a64d-63dbf452d900}</x14:id>
+          <x14:id>{f66f4807-f532-4f9c-ab81-cf62f19f1935}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12324,7 +12324,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{07918e4e-05c3-42e5-b0eb-8791d0e32c89}</x14:id>
+          <x14:id>{13df11c4-5186-4004-8442-7103a27e7028}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12343,7 +12343,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{387ed673-6671-4b7e-beb1-84a44683f713}</x14:id>
+          <x14:id>{b90d7521-a96e-434b-b021-e551441590e4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12365,7 +12365,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{342bbaae-92d3-45d2-b1fe-8bf9fd3084ec}</x14:id>
+          <x14:id>{5055c290-299e-4fa6-8736-dcd01f5a40e7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12416,7 +12416,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{aa11a8f2-eb39-4805-b857-351575796bf6}">
+          <x14:cfRule type="dataBar" id="{ffe80b8e-6d0e-4556-97a8-da7ee6b14e3a}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12431,7 +12431,7 @@
           <xm:sqref>D85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{befd2a02-8225-4779-bee9-4a7436c8581b}">
+          <x14:cfRule type="dataBar" id="{1a09c170-6c36-449a-9635-45663dcefaa0}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12446,7 +12446,7 @@
           <xm:sqref>D67:D84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f5b9f4de-06fd-441a-b84c-d9e8a27b23a3}">
+          <x14:cfRule type="dataBar" id="{3c34237c-1a35-44c0-870d-3b59b76cdda3}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12461,7 +12461,7 @@
           <xm:sqref>D86:D97</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{827e6eec-407e-4811-a64d-63dbf452d900}">
+          <x14:cfRule type="dataBar" id="{f66f4807-f532-4f9c-ab81-cf62f19f1935}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12476,7 +12476,7 @@
           <xm:sqref>D98:D99</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{07918e4e-05c3-42e5-b0eb-8791d0e32c89}">
+          <x14:cfRule type="dataBar" id="{13df11c4-5186-4004-8442-7103a27e7028}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12491,7 +12491,7 @@
           <xm:sqref>D100:D117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{387ed673-6671-4b7e-beb1-84a44683f713}">
+          <x14:cfRule type="dataBar" id="{b90d7521-a96e-434b-b021-e551441590e4}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12506,7 +12506,7 @@
           <xm:sqref>D7:D65 D126:D127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{342bbaae-92d3-45d2-b1fe-8bf9fd3084ec}">
+          <x14:cfRule type="dataBar" id="{5055c290-299e-4fa6-8736-dcd01f5a40e7}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Hoan thanh Activity Bar Chart
</commit_message>
<xml_diff>
--- a/Bao cao/Activity Bar Chart.xlsx
+++ b/Bao cao/Activity Bar Chart.xlsx
@@ -352,40 +352,40 @@
     <t>Giai đoạn 7: Thiết kế State Machine Diagram</t>
   </si>
   <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý nhân viên</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý ca làm nhân viên</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng cấp tài khoản nhân viên</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý chức vụ</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng tiếp nhận khách hàng</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý tủ đồ</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý sản phẩm</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng giữ trả xe</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý nhập hàng</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý xuất hàng</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng quản lý hóa đơn</t>
-  </si>
-  <si>
-    <t>Vẽ State Machine Diagram của chức năng tổ chức khuyến mãi</t>
+    <t>Vẽ State Machine Diagram của nhân viên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vẽ State Machine Diagram của ca </t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của tài khoản nhân viên</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của chức vụ</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của khách hàng</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của tủ đồ</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của sản phẩm</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của thẻ xe</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của phiếu nhập</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của phiếu xuất</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của hóa đơn</t>
+  </si>
+  <si>
+    <t>Vẽ State Machine Diagram của chương trình khuyến mãi</t>
   </si>
   <si>
     <t>Giai đoạn 8: Thiết kế Usecase</t>
@@ -504,13 +504,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="180" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="179" formatCode="ddd\,\ m/d/yyyy"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="d"/>
   </numFmts>
   <fonts count="47">
@@ -707,7 +707,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -715,7 +715,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,13 +737,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -758,11 +751,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -776,29 +769,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -826,9 +804,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -837,6 +822,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -976,19 +976,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,7 +1000,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,7 +1042,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,7 +1078,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,61 +1090,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,16 +1240,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1259,15 +1259,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1288,27 +1279,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1330,22 +1328,24 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1355,131 +1355,131 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="41" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="28" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1545,10 +1545,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1572,10 +1572,10 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1590,10 +1590,10 @@
     <xf numFmtId="9" fontId="15" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1605,10 +1605,10 @@
     <xf numFmtId="9" fontId="15" fillId="4" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="4" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1623,10 +1623,10 @@
     <xf numFmtId="9" fontId="15" fillId="5" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1638,10 +1638,10 @@
     <xf numFmtId="9" fontId="15" fillId="6" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="6" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1656,10 +1656,10 @@
     <xf numFmtId="9" fontId="15" fillId="7" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1671,10 +1671,10 @@
     <xf numFmtId="9" fontId="15" fillId="8" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1686,10 +1686,10 @@
     <xf numFmtId="9" fontId="15" fillId="9" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1701,10 +1701,10 @@
     <xf numFmtId="9" fontId="15" fillId="10" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1716,10 +1716,10 @@
     <xf numFmtId="9" fontId="15" fillId="11" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1731,10 +1731,10 @@
     <xf numFmtId="9" fontId="15" fillId="12" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1743,13 +1743,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="181" fontId="19" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1779,10 +1779,10 @@
     <xf numFmtId="9" fontId="15" fillId="15" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1794,10 +1794,10 @@
     <xf numFmtId="9" fontId="15" fillId="16" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1809,10 +1809,10 @@
     <xf numFmtId="9" fontId="15" fillId="17" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1824,10 +1824,10 @@
     <xf numFmtId="9" fontId="15" fillId="18" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1839,10 +1839,10 @@
     <xf numFmtId="9" fontId="15" fillId="19" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="12" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1857,10 +1857,10 @@
     <xf numFmtId="9" fontId="15" fillId="20" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="20" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="22" fillId="20" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="20" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="20" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="20" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2466,9 +2466,9 @@
   <dimension ref="A1:BL131"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="$A94:$XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -12268,7 +12268,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ffe80b8e-6d0e-4556-97a8-da7ee6b14e3a}</x14:id>
+          <x14:id>{0ca29208-548b-49a0-8225-7b32bfcdf64a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12282,7 +12282,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1a09c170-6c36-449a-9635-45663dcefaa0}</x14:id>
+          <x14:id>{879844fa-c45f-4298-b56d-12fa9f639371}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12296,7 +12296,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3c34237c-1a35-44c0-870d-3b59b76cdda3}</x14:id>
+          <x14:id>{3103410c-4b71-40e3-ae7a-5cd51b435950}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12310,7 +12310,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f66f4807-f532-4f9c-ab81-cf62f19f1935}</x14:id>
+          <x14:id>{d75bb1fe-420d-4a43-9ebb-fe4defc9ea2d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12324,7 +12324,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{13df11c4-5186-4004-8442-7103a27e7028}</x14:id>
+          <x14:id>{0fb05e5f-d664-4033-97ef-99d48ec575f4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12343,7 +12343,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b90d7521-a96e-434b-b021-e551441590e4}</x14:id>
+          <x14:id>{5d910037-563f-4143-9806-535f4a3eaf03}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12365,7 +12365,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5055c290-299e-4fa6-8736-dcd01f5a40e7}</x14:id>
+          <x14:id>{91d9b741-85f5-4685-9dba-7393afbeab49}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12416,7 +12416,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ffe80b8e-6d0e-4556-97a8-da7ee6b14e3a}">
+          <x14:cfRule type="dataBar" id="{0ca29208-548b-49a0-8225-7b32bfcdf64a}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12431,7 +12431,7 @@
           <xm:sqref>D85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1a09c170-6c36-449a-9635-45663dcefaa0}">
+          <x14:cfRule type="dataBar" id="{879844fa-c45f-4298-b56d-12fa9f639371}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12446,7 +12446,7 @@
           <xm:sqref>D67:D84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3c34237c-1a35-44c0-870d-3b59b76cdda3}">
+          <x14:cfRule type="dataBar" id="{3103410c-4b71-40e3-ae7a-5cd51b435950}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12461,7 +12461,7 @@
           <xm:sqref>D86:D97</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f66f4807-f532-4f9c-ab81-cf62f19f1935}">
+          <x14:cfRule type="dataBar" id="{d75bb1fe-420d-4a43-9ebb-fe4defc9ea2d}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12476,7 +12476,7 @@
           <xm:sqref>D98:D99</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{13df11c4-5186-4004-8442-7103a27e7028}">
+          <x14:cfRule type="dataBar" id="{0fb05e5f-d664-4033-97ef-99d48ec575f4}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12491,7 +12491,7 @@
           <xm:sqref>D100:D117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b90d7521-a96e-434b-b021-e551441590e4}">
+          <x14:cfRule type="dataBar" id="{5d910037-563f-4143-9806-535f4a3eaf03}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12506,7 +12506,7 @@
           <xm:sqref>D7:D65 D126:D127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5055c290-299e-4fa6-8736-dcd01f5a40e7}">
+          <x14:cfRule type="dataBar" id="{91d9b741-85f5-4685-9dba-7393afbeab49}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>